<commit_message>
There is new version of article, all tests done on ATI Radeon HD4890 and NVIDIA QUADRO FX5600. From Article was deleted information about CPU.
</commit_message>
<xml_diff>
--- a/NChargesTestsResults.xlsx
+++ b/NChargesTestsResults.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>AMD Athlon 3800+</t>
   </si>
@@ -57,6 +56,24 @@
   <si>
     <t>G92</t>
   </si>
+  <si>
+    <t>ATI Radeon HD4890</t>
+  </si>
+  <si>
+    <t>Shaders</t>
+  </si>
+  <si>
+    <t>Nvidia Quadro FX5600</t>
+  </si>
+  <si>
+    <t>Cuda</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>GFLOPS</t>
+  </si>
 </sst>
 </file>
 
@@ -80,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -103,11 +120,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -125,6 +171,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -401,12 +469,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="88194432"/>
-        <c:axId val="88414080"/>
+        <c:axId val="57437568"/>
+        <c:axId val="57447936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88194432"/>
+        <c:axId val="57437568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,14 +499,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88414080"/>
+        <c:crossAx val="57447936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88414080"/>
+        <c:axId val="57447936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +532,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88194432"/>
+        <c:crossAx val="57437568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -478,7 +545,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -585,7 +652,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
           <c:bubble3D val="1"/>
         </c:ser>
         <c:ser>
@@ -662,7 +728,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
           <c:bubble3D val="1"/>
         </c:ser>
         <c:ser>
@@ -739,7 +804,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
           <c:bubble3D val="1"/>
         </c:ser>
         <c:ser>
@@ -816,15 +880,13 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="1"/>
           <c:bubble3D val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="88458752"/>
-        <c:axId val="88460288"/>
+        <c:axId val="57390592"/>
+        <c:axId val="57392512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88458752"/>
+        <c:axId val="57390592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,14 +913,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88460288"/>
+        <c:crossAx val="57392512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88460288"/>
+        <c:axId val="57392512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +947,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88458752"/>
+        <c:crossAx val="57390592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -898,7 +960,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1254,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1270,10 +1332,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
@@ -1443,16 +1505,16 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
@@ -1621,17 +1683,17 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:8">
+      <c r="A33" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="D33" s="8" t="s">
+      <c r="B33" s="10"/>
+      <c r="D33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:8">
       <c r="A35" s="2">
         <v>96</v>
       </c>
@@ -1659,7 +1721,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:8">
       <c r="A37" s="2">
         <v>256</v>
       </c>
@@ -1675,7 +1737,7 @@
         <v>150792.73897058822</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:8">
       <c r="A38" s="2">
         <f>A37*2</f>
         <v>512</v>
@@ -1693,9 +1755,9 @@
         <v>37698.184742647056</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:8">
       <c r="A39" s="2">
-        <f t="shared" ref="A39:A45" si="6">A38*2</f>
+        <f t="shared" ref="A39:A43" si="6">A38*2</f>
         <v>1024</v>
       </c>
       <c r="B39" s="2">
@@ -1711,7 +1773,7 @@
         <v>9424.546185661764</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:8">
       <c r="A40" s="2">
         <f t="shared" si="6"/>
         <v>2048</v>
@@ -1729,7 +1791,7 @@
         <v>2356.136546415441</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:8">
       <c r="A41" s="2">
         <f t="shared" si="6"/>
         <v>4096</v>
@@ -1747,7 +1809,7 @@
         <v>589.03413660386025</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:8">
       <c r="A42" s="2">
         <f t="shared" si="6"/>
         <v>8192</v>
@@ -1765,7 +1827,7 @@
         <v>147.25853415096506</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:8">
       <c r="A43" s="2">
         <f t="shared" si="6"/>
         <v>16384</v>
@@ -1783,8 +1845,288 @@
         <v>36.814633537741265</v>
       </c>
     </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="E46" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="15"/>
+      <c r="B47" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="2"/>
+      <c r="B48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="2">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="B49" s="2">
+        <v>316</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3108</v>
+      </c>
+      <c r="E49" s="2">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1147.7</v>
+      </c>
+      <c r="G49" s="2">
+        <v>907.6</v>
+      </c>
+      <c r="H49" s="2">
+        <f>(H54*1000*1000*1000)/(E49*E49*20)</f>
+        <v>1398.003101348877</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="2">
+        <f t="shared" ref="A50:A52" si="8">A49*2</f>
+        <v>4096</v>
+      </c>
+      <c r="B50" s="2">
+        <v>152.9</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1617</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" ref="E50:E52" si="9">E49*2</f>
+        <v>4096</v>
+      </c>
+      <c r="F50" s="2">
+        <v>583.79999999999995</v>
+      </c>
+      <c r="G50" s="2">
+        <v>319.89999999999998</v>
+      </c>
+      <c r="H50" s="2">
+        <f>(H55*1000*1000*1000)/(E50*E50*20)</f>
+        <v>672.19138145446777</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="2">
+        <f t="shared" si="8"/>
+        <v>8192</v>
+      </c>
+      <c r="B51" s="2">
+        <v>67.3</v>
+      </c>
+      <c r="C51" s="2">
+        <v>392.2</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="9"/>
+        <v>8192</v>
+      </c>
+      <c r="F51" s="2">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="G51" s="2">
+        <v>106.9</v>
+      </c>
+      <c r="H51" s="2">
+        <f>(H56*1000*1000*1000)/(E51*E51*20)</f>
+        <v>172.44964838027954</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="2">
+        <f t="shared" si="8"/>
+        <v>16384</v>
+      </c>
+      <c r="B52" s="2">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="C52" s="2">
+        <v>106.9</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="9"/>
+        <v>16384</v>
+      </c>
+      <c r="F52" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="G52" s="2">
+        <v>27.8</v>
+      </c>
+      <c r="H52" s="2">
+        <f>(H57*1000*1000*1000)/(E52*E52*20)</f>
+        <v>43.396465480327606</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="B53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="2">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="B54" s="2">
+        <f>(B49*A54*A54*20)/(1000*1000*1000)</f>
+        <v>26.508001279999998</v>
+      </c>
+      <c r="C54" s="2">
+        <f>(C49*A54*A54*20)/(1000*1000*1000)</f>
+        <v>260.71793664</v>
+      </c>
+      <c r="E54" s="2">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="F54" s="2">
+        <f>(F49*E54*E54*20)/(1000*1000*1000)</f>
+        <v>96.276054016000003</v>
+      </c>
+      <c r="G54" s="2">
+        <f>(G49*E54*E54*20)/(1000*1000*1000)</f>
+        <v>76.135006207999993</v>
+      </c>
+      <c r="H54" s="2">
+        <v>117.273</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="2">
+        <f t="shared" ref="A55:A57" si="10">A54*2</f>
+        <v>4096</v>
+      </c>
+      <c r="B55" s="2">
+        <f t="shared" ref="B55:B57" si="11">(B50*A55*A55*20)/(1000*1000*1000)</f>
+        <v>51.304726528000003</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" ref="C55:C57" si="12">(C50*A55*A55*20)/(1000*1000*1000)</f>
+        <v>542.57516543999998</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" ref="E55:E57" si="13">E54*2</f>
+        <v>4096</v>
+      </c>
+      <c r="F55" s="2">
+        <f t="shared" ref="F55:F57" si="14">(F50*E55*E55*20)/(1000*1000*1000)</f>
+        <v>195.89077401599999</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" ref="G55:G57" si="15">(G50*E55*E55*20)/(1000*1000*1000)</f>
+        <v>107.34062796800001</v>
+      </c>
+      <c r="H55" s="2">
+        <v>225.55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="2">
+        <f t="shared" si="10"/>
+        <v>8192</v>
+      </c>
+      <c r="B56" s="2">
+        <f t="shared" si="11"/>
+        <v>90.328530943999993</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="12"/>
+        <v>526.40192921599998</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="13"/>
+        <v>8192</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="14"/>
+        <v>199.044890624</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="15"/>
+        <v>143.47875123200001</v>
+      </c>
+      <c r="H56" s="2">
+        <v>231.458</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="2">
+        <f t="shared" si="10"/>
+        <v>16384</v>
+      </c>
+      <c r="B57" s="2">
+        <f t="shared" si="11"/>
+        <v>90.731184127999995</v>
+      </c>
+      <c r="C57" s="2">
+        <f t="shared" si="12"/>
+        <v>573.91500492800003</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="13"/>
+        <v>16384</v>
+      </c>
+      <c r="F57" s="2">
+        <f t="shared" si="14"/>
+        <v>200.25285017600001</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="15"/>
+        <v>149.25011353599999</v>
+      </c>
+      <c r="H57" s="2">
+        <v>232.983</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E53:H53"/>
+    <mergeCell ref="E46:H46"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A17:B17"/>

</xml_diff>